<commit_message>
Upload new Main Edge Cut and other things
</commit_message>
<xml_diff>
--- a/PCB/MK I/FL-Zetor Součástky.xlsx
+++ b/PCB/MK I/FL-Zetor Součástky.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vadim\GitHub\Bobutek-LineFollower\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vadim\GitHub\Bobutek-LineFollower\PCB\MK I\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1866B643-BF90-444D-944E-B47687D4B7CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{019AD688-5DDA-4B04-BE9E-E46F76530DEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4373ECF8-08D4-4232-8CEF-8C0BA3D5B12B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>Name</t>
   </si>
@@ -75,6 +75,15 @@
   </si>
   <si>
     <t>StepDown - GME</t>
+  </si>
+  <si>
+    <t>LM1086</t>
+  </si>
+  <si>
+    <t>TO-220</t>
+  </si>
+  <si>
+    <t>LM1086 Stab. 5v - Mouser</t>
   </si>
 </sst>
 </file>
@@ -497,10 +506,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8D12BA8-1A6C-4B76-87D2-96E4C19A408C}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -536,7 +545,7 @@
         <v>4</v>
       </c>
       <c r="D2" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -572,6 +581,20 @@
         <v>12</v>
       </c>
       <c r="D5" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="1">
         <v>1</v>
       </c>
     </row>
@@ -580,6 +603,7 @@
     <hyperlink ref="C2" r:id="rId1" display="https://www.laskakit.cz/user/related_files/tb6612fng_datasheet_en_20141001.pdf" xr:uid="{4689D627-A470-44F3-993D-21C14D7B8052}"/>
     <hyperlink ref="C4" r:id="rId2" xr:uid="{651789BD-4C7B-437F-ACFF-F511B9707874}"/>
     <hyperlink ref="C5" r:id="rId3" xr:uid="{C82F9D65-4C45-4E54-8083-FF9A2AE8D64B}"/>
+    <hyperlink ref="C6" r:id="rId4" xr:uid="{4F6E53D2-4C7C-4709-B801-C88D9BE26A81}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>